<commit_message>
Added London environment data
</commit_message>
<xml_diff>
--- a/viz/London_Neighbors.xlsx
+++ b/viz/London_Neighbors.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8100" windowHeight="10114"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8100" windowHeight="10110" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="London_Nearest_Neighbor" sheetId="1" r:id="rId1"/>
+    <sheet name="London_Enviornment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>aq_station</t>
   </si>
@@ -132,6 +133,33 @@
   </si>
   <si>
     <t>london_grid_366</t>
+  </si>
+  <si>
+    <t>station_id</t>
+  </si>
+  <si>
+    <t>terrain</t>
+  </si>
+  <si>
+    <t>landclass</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>suburbs</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>industrial</t>
   </si>
 </sst>
 </file>
@@ -485,16 +513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="19.3046875" customWidth="1"/>
+    <col min="1" max="2" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -510,7 +538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -518,7 +546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -526,7 +554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -534,7 +562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -542,7 +570,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -550,7 +578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -558,7 +586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -566,7 +594,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -574,7 +602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -582,7 +610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -590,7 +618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -598,7 +626,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -606,7 +634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -614,7 +642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -622,7 +650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -630,7 +658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -638,7 +666,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -646,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -654,7 +682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -662,7 +690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -670,7 +698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -678,7 +706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -686,7 +714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -697,4 +725,412 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A26:A35">
+    <sortCondition ref="A26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>